<commit_message>
docs: Changed information on Configuration file
</commit_message>
<xml_diff>
--- a/MainProcess/Data/Config.xlsx
+++ b/MainProcess/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/43a1c60308be9d09/Documentos/UiPath/PwC_Test/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\ReFramework-WordIndexes\MainProcess\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{9BE7DFF5-5AFC-4110-8461-609B0BDD5551}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{CBC0D5C9-B2B9-4BA8-8CC7-F980E94FF8AC}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DC808B5-471F-4683-BF82-112D8A31F90D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2295" yWindow="2295" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -120,7 +120,7 @@
     <t>OrchestratorAssetFolder</t>
   </si>
   <si>
-    <t>PwC_BL</t>
+    <t>BE_Queue</t>
   </si>
 </sst>
 </file>
@@ -499,7 +499,7 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>